<commit_message>
Generate visualizations from the data
</commit_message>
<xml_diff>
--- a/customer_feedback_with_sentiment_and_aspects.xlsx
+++ b/customer_feedback_with_sentiment_and_aspects.xlsx
@@ -1474,7 +1474,7 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Positive</t>
+          <t>Neutral</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Neutral</t>
+          <t>Positive</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">

</xml_diff>